<commit_message>
In Simulationen 9_1_2 ausgeben lassen der Strombedarfe der einzelnen WP u
und anlegen der Auswertungen
</commit_message>
<xml_diff>
--- a/9_kaltes_Nahwaermenetz/9_1_2_Kosten/9_1_2_Kosten_10.xlsx
+++ b/9_kaltes_Nahwaermenetz/9_1_2_Kosten/9_1_2_Kosten_10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fraunhofer-my.sharepoint.com/personal/lara_josephine_barnic_iee_fraunhofer_de/Documents/A_Bearbeitung/9_Parameterstudie_REP/9_kaltes_Nahwaermenetz/9_1_2_Kosten/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1585" documentId="11_AD4DB114E441178AC67DF4879E90C19A693EDF21" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39EC901B-E470-48C0-8660-A59FA9406240}"/>
+  <xr:revisionPtr revIDLastSave="1590" documentId="11_AD4DB114E441178AC67DF4879E90C19A693EDF21" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A70A135D-9F69-4719-B601-A4E89238FEEE}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zusammenfassung" sheetId="8" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="128">
   <si>
     <t>Investitionskosten</t>
   </si>
@@ -449,6 +449,9 @@
   </si>
   <si>
     <t xml:space="preserve">Speicher, 20.500 l </t>
+  </si>
+  <si>
+    <t>SW-WP</t>
   </si>
 </sst>
 </file>
@@ -1129,7 +1132,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DBA93AF5-0303-4BA4-8D74-229DEDBDAFA5}" type="CELLRANGE">
+                    <a:fld id="{1389F948-F03A-4AD2-8C99-6DCAF06D4E5F}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -1163,7 +1166,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{16A9E320-08E1-4A71-87AE-8C4BD1E5DBBA}" type="CELLRANGE">
+                    <a:fld id="{81019E9E-19B8-466A-8307-3F8B62958536}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -1245,7 +1248,7 @@
                   <c:v>1.7784505465183746</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)">
-                  <c:v>2.1491305344827358</c:v>
+                  <c:v>2.2267961944827359</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1677,7 +1680,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{05A663A1-E5CA-498A-AF3E-13C97DA0D570}" type="CELLRANGE">
+                    <a:fld id="{B14E715D-BE55-4249-AE8E-85008B32DC40}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -1711,7 +1714,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{57569412-27C9-41F9-8A05-6C1F50A690CF}" type="CELLRANGE">
+                    <a:fld id="{9D500189-A6AE-463C-B240-FB11231707AB}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -1793,7 +1796,7 @@
                   <c:v>1.7784505465183746</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)">
-                  <c:v>2.1491305344827358</c:v>
+                  <c:v>2.2267961944827359</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2383,7 +2386,7 @@
                   <c:v>247848</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>243744</c:v>
+                  <c:v>257469.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>251901.11850488459</c:v>
@@ -2832,7 +2835,7 @@
                   <c:v>0.76343974359810018</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.73518103002537394</c:v>
+                  <c:v>0.73051543080244696</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.35424094374360549</c:v>
@@ -2897,7 +2900,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.5158058730944549E-2</c:v>
+                  <c:v>4.4871477065858992E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.16650881084100905</c:v>
@@ -2962,7 +2965,7 @@
                   <c:v>0.11975760352614045</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.11341516771044603</c:v>
+                  <c:v>0.11904160437795122</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.14164077769720654</c:v>
@@ -3027,7 +3030,7 @@
                   <c:v>9.3851141596702589E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.2854267504799841E-2</c:v>
+                  <c:v>7.239192040935645E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.32443788977025201</c:v>
@@ -3092,7 +3095,7 @@
                   <c:v>2.2951511279056806E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.3391476028435667E-2</c:v>
+                  <c:v>3.3179567344386408E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.3171577947926918E-2</c:v>
@@ -5734,6 +5737,10 @@
 </externalLink>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -6040,7 +6047,7 @@
       </c>
       <c r="D2" s="42">
         <f t="shared" si="0"/>
-        <v>2.1491305344827358</v>
+        <v>2.2267961944827359</v>
       </c>
       <c r="F2" s="2">
         <v>1000000</v>
@@ -6118,26 +6125,26 @@
         <v>1778450.5465183747</v>
       </c>
       <c r="D5" s="42">
-        <f>'kalte NW'!B31</f>
-        <v>2149130.5344827357</v>
+        <f>'kalte NW'!B32</f>
+        <v>2226796.1944827358</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>49</v>
       </c>
       <c r="K5" s="42">
         <f>D2</f>
-        <v>2.1491305344827358</v>
+        <v>2.2267961944827359</v>
       </c>
       <c r="L5" s="42">
         <v>243.30137300000001</v>
       </c>
       <c r="M5" s="3">
         <f>(K5-K4)/K4</f>
-        <v>0.20842861708470417</v>
+        <v>0.25209902453687882</v>
       </c>
       <c r="N5" s="3">
         <f>K5-K4</f>
-        <v>0.37067998796436119</v>
+        <v>0.44834564796436127</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
@@ -6160,11 +6167,11 @@
       </c>
       <c r="D7" s="3">
         <f>D5-C5</f>
-        <v>370679.98796436097</v>
+        <v>448345.64796436112</v>
       </c>
       <c r="F7" s="3">
         <f>D2-C2</f>
-        <v>0.37067998796436119</v>
+        <v>0.44834564796436127</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
@@ -6177,7 +6184,7 @@
       </c>
       <c r="D8" s="45">
         <f>D7/C5</f>
-        <v>0.20842861708470406</v>
+        <v>0.25209902453687871</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3">
@@ -6259,7 +6266,7 @@
       </c>
       <c r="D15">
         <f>D2/D14</f>
-        <v>6.429327840456662E-4</v>
+        <v>6.6616720289894564E-4</v>
       </c>
     </row>
   </sheetData>
@@ -6340,8 +6347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2B24C0F-6734-4579-B89E-086B8618A834}">
   <dimension ref="B1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7740,7 +7747,7 @@
         <v>dezentral</v>
       </c>
       <c r="C2" s="42" t="str" cm="1">
-        <f t="array" ref="C2:C9">'kalte NW'!C33:C40</f>
+        <f t="array" ref="C2:C9">'kalte NW'!C34:C41</f>
         <v>KNW</v>
       </c>
       <c r="D2" s="42" t="str" cm="1">
@@ -7787,7 +7794,7 @@
       </c>
       <c r="J3" s="2">
         <f t="shared" si="0"/>
-        <v>0.73518103002537394</v>
+        <v>0.73051543080244696</v>
       </c>
       <c r="K3" s="2">
         <f t="shared" si="0"/>
@@ -7820,7 +7827,7 @@
       </c>
       <c r="J4" s="2">
         <f t="shared" si="0"/>
-        <v>4.5158058730944549E-2</v>
+        <v>4.4871477065858992E-2</v>
       </c>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
@@ -7835,7 +7842,7 @@
         <v>247848</v>
       </c>
       <c r="C5" s="2">
-        <v>243744</v>
+        <v>257469.9</v>
       </c>
       <c r="D5" s="2">
         <v>251901.11850488459</v>
@@ -7853,7 +7860,7 @@
       </c>
       <c r="J5" s="2">
         <f t="shared" si="0"/>
-        <v>0.11341516771044603</v>
+        <v>0.11904160437795122</v>
       </c>
       <c r="K5" s="2">
         <f t="shared" si="0"/>
@@ -7886,7 +7893,7 @@
       </c>
       <c r="J6" s="2">
         <f t="shared" si="0"/>
-        <v>7.2854267504799841E-2</v>
+        <v>7.239192040935645E-2</v>
       </c>
       <c r="K6" s="2">
         <f t="shared" si="0"/>
@@ -7919,7 +7926,7 @@
       </c>
       <c r="J7" s="2">
         <f t="shared" si="0"/>
-        <v>3.3391476028435667E-2</v>
+        <v>3.3179567344386408E-2</v>
       </c>
       <c r="K7" s="2">
         <f t="shared" si="0"/>
@@ -7946,7 +7953,7 @@
         <v>2069580.4917797993</v>
       </c>
       <c r="C9" s="2">
-        <v>2149130.5344827357</v>
+        <v>2162856.4344827356</v>
       </c>
       <c r="D9" s="2">
         <v>1778450.5465183747</v>
@@ -7971,7 +7978,7 @@
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C10" s="2">
         <f>C9-B9</f>
-        <v>79550.042702936335</v>
+        <v>93275.942702936241</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
@@ -7999,7 +8006,7 @@
       </c>
       <c r="D12" s="46">
         <f>ROUND(C9,-4)</f>
-        <v>2150000</v>
+        <v>2160000</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
@@ -8106,7 +8113,7 @@
         <v>247848</v>
       </c>
       <c r="D37" s="2">
-        <v>243744</v>
+        <v>257469.9</v>
       </c>
       <c r="E37" s="2">
         <v>251901.11850488459</v>
@@ -8721,10 +8728,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FE05C22-774F-487B-8758-21CEEC91D1E4}">
-  <dimension ref="A1:S42"/>
+  <dimension ref="A1:S43"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8846,11 +8853,10 @@
       </c>
       <c r="C6" s="52">
         <f>D6*E6</f>
-        <v>94164</v>
+        <v>120452.4</v>
       </c>
       <c r="D6" s="4">
-        <f>[2]K_NW!$F$10</f>
-        <v>82.6</v>
+        <v>105.66</v>
       </c>
       <c r="E6" s="25">
         <v>1140</v>
@@ -9037,10 +9043,10 @@
       </c>
       <c r="C16" s="52">
         <f>D16*E16</f>
-        <v>27600</v>
+        <v>22770</v>
       </c>
       <c r="D16">
-        <v>20</v>
+        <v>16.5</v>
       </c>
       <c r="E16" s="25">
         <v>1380</v>
@@ -9067,11 +9073,11 @@
         <v>28</v>
       </c>
       <c r="C17" s="52">
-        <f t="shared" ref="C17:C19" si="0">D17*E17</f>
-        <v>43350</v>
+        <f t="shared" ref="C17:C20" si="0">D17*E17</f>
+        <v>39708.6</v>
       </c>
       <c r="D17">
-        <v>50</v>
+        <v>45.8</v>
       </c>
       <c r="E17" s="25">
         <v>867</v>
@@ -9099,10 +9105,10 @@
       </c>
       <c r="C18" s="52">
         <f t="shared" si="0"/>
-        <v>51030</v>
+        <v>58392.899999999994</v>
       </c>
       <c r="D18">
-        <v>70</v>
+        <v>80.099999999999994</v>
       </c>
       <c r="E18" s="25">
         <v>729</v>
@@ -9130,10 +9136,10 @@
       </c>
       <c r="C19" s="52">
         <f t="shared" si="0"/>
-        <v>27600</v>
+        <v>16145.999999999998</v>
       </c>
       <c r="D19">
-        <v>20</v>
+        <v>11.7</v>
       </c>
       <c r="E19" s="25">
         <v>1380</v>
@@ -9156,38 +9162,53 @@
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="53" t="s">
+        <v>127</v>
+      </c>
+      <c r="C20" s="52">
+        <f t="shared" si="0"/>
+        <v>63939.759999999995</v>
+      </c>
+      <c r="D20">
+        <v>112.57</v>
+      </c>
+      <c r="E20" s="25">
+        <v>568</v>
+      </c>
+      <c r="F20" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="I20" s="7"/>
+      <c r="K20"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B21" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C21" s="9" t="s">
         <v>5</v>
-      </c>
-      <c r="G20" s="20"/>
-      <c r="K20"/>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B21" s="72">
-        <f>SUM(C16:C19)</f>
-        <v>149580</v>
       </c>
       <c r="G21" s="20"/>
       <c r="K21"/>
-      <c r="O21">
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B22" s="72">
+        <f>SUM(C16:C19)</f>
+        <v>137017.5</v>
+      </c>
+      <c r="G22" s="20"/>
+      <c r="K22"/>
+      <c r="O22">
         <f>SUM(O16:O19)</f>
         <v>160</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B22" s="58" t="s">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B23" s="58" t="s">
         <v>7</v>
-      </c>
-      <c r="C22" s="59"/>
-      <c r="G22" s="20"/>
-      <c r="K22"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B23" s="60" t="s">
-        <v>121</v>
       </c>
       <c r="C23" s="59"/>
       <c r="G23" s="20"/>
@@ -9195,89 +9216,80 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B24" s="60" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="59">
-        <v>420000</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="C24" s="59"/>
       <c r="G24" s="20"/>
       <c r="K24"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B25" s="60" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C25" s="59">
-        <v>170000</v>
+        <v>420000</v>
       </c>
       <c r="G25" s="20"/>
       <c r="K25"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B26" s="60" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C26" s="59">
-        <v>790000</v>
+        <v>170000</v>
       </c>
       <c r="G26" s="20"/>
       <c r="K26"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B27" s="60" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C27" s="59">
-        <v>200000</v>
+        <v>790000</v>
       </c>
       <c r="G27" s="20"/>
       <c r="K27"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B28" s="60" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="59">
+        <v>200000</v>
+      </c>
       <c r="G28" s="20"/>
-      <c r="H28" t="s">
-        <v>78</v>
-      </c>
-      <c r="I28" s="39">
-        <f>SUM(I5:I27)</f>
-        <v>2870.5056289663762</v>
-      </c>
       <c r="K28"/>
     </row>
-    <row r="29" spans="1:19" s="27" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="19"/>
-      <c r="C29" s="6"/>
-      <c r="D29"/>
-      <c r="E29"/>
-      <c r="F29"/>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
       <c r="G29" s="20"/>
       <c r="H29" t="s">
+        <v>78</v>
+      </c>
+      <c r="I29" s="39">
+        <f>SUM(I5:I28)</f>
+        <v>2870.5056289663762</v>
+      </c>
+      <c r="K29"/>
+    </row>
+    <row r="30" spans="1:19" s="27" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B30" s="19"/>
+      <c r="C30" s="6"/>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30"/>
+      <c r="G30" s="20"/>
+      <c r="H30" t="s">
         <v>79</v>
       </c>
-      <c r="I29" s="8">
-        <f>I28*'Allgemeine Parameter'!C3</f>
+      <c r="I30" s="8">
+        <f>I29*'Allgemeine Parameter'!C3</f>
         <v>71762.640724159399</v>
       </c>
-      <c r="J29"/>
-      <c r="K29"/>
-      <c r="L29" s="6"/>
-      <c r="M29"/>
-      <c r="N29"/>
-      <c r="O29"/>
-      <c r="P29"/>
-      <c r="Q29"/>
-      <c r="R29"/>
-      <c r="S29"/>
-    </row>
-    <row r="30" spans="1:19" s="31" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="30"/>
-      <c r="B30" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="10"/>
-      <c r="G30" s="32"/>
-      <c r="I30" s="5"/>
-      <c r="L30" s="5"/>
+      <c r="J30"/>
+      <c r="K30"/>
+      <c r="L30" s="6"/>
       <c r="M30"/>
       <c r="N30"/>
       <c r="O30"/>
@@ -9286,25 +9298,15 @@
       <c r="R30"/>
       <c r="S30"/>
     </row>
-    <row r="31" spans="1:19" s="27" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="28"/>
-      <c r="B31" s="33">
-        <f>SUM(C31,I31,L31)</f>
-        <v>2149130.5344827357</v>
-      </c>
-      <c r="C31" s="17">
-        <f>SUM(C1:C28)</f>
-        <v>1920794.5628966377</v>
-      </c>
-      <c r="G31" s="29"/>
-      <c r="I31" s="57">
-        <f>SUM(I29)</f>
-        <v>71762.640724159399</v>
-      </c>
-      <c r="L31" s="54">
-        <f>SUM(L5:L6)</f>
-        <v>156573.33086193868</v>
-      </c>
+    <row r="31" spans="1:19" s="31" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="30"/>
+      <c r="B31" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="10"/>
+      <c r="G31" s="32"/>
+      <c r="I31" s="5"/>
+      <c r="L31" s="5"/>
       <c r="M31"/>
       <c r="N31"/>
       <c r="O31"/>
@@ -9313,110 +9315,132 @@
       <c r="R31"/>
       <c r="S31"/>
     </row>
-    <row r="32" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B32"/>
-      <c r="C32" s="34"/>
-      <c r="I32"/>
-      <c r="K32"/>
-      <c r="L32"/>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B33" s="61" t="s">
-        <v>110</v>
-      </c>
-      <c r="C33" s="62" t="s">
-        <v>111</v>
-      </c>
+    <row r="32" spans="1:19" s="27" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="28"/>
+      <c r="B32" s="33">
+        <f>SUM(C32,I32,L32)</f>
+        <v>2226796.1944827358</v>
+      </c>
+      <c r="C32" s="17">
+        <f>SUM(C1:C29)</f>
+        <v>1998460.2228966376</v>
+      </c>
+      <c r="G32" s="29"/>
+      <c r="I32" s="57">
+        <f>SUM(I30)</f>
+        <v>71762.640724159399</v>
+      </c>
+      <c r="L32" s="54">
+        <f>SUM(L5:L6)</f>
+        <v>156573.33086193868</v>
+      </c>
+      <c r="M32"/>
+      <c r="N32"/>
+      <c r="O32"/>
+      <c r="P32"/>
+      <c r="Q32"/>
+      <c r="R32"/>
+      <c r="S32"/>
+    </row>
+    <row r="33" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B33"/>
+      <c r="C33" s="34"/>
       <c r="I33"/>
       <c r="K33"/>
       <c r="L33"/>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B34" s="60" t="s">
-        <v>105</v>
-      </c>
-      <c r="C34" s="63">
-        <f>SUM(C24:C27)</f>
-        <v>1580000</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F34" s="25"/>
-      <c r="H34" s="3"/>
+      <c r="B34" s="61" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" s="62" t="s">
+        <v>111</v>
+      </c>
       <c r="I34"/>
       <c r="K34"/>
       <c r="L34"/>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B35" s="49" t="s">
-        <v>107</v>
-      </c>
-      <c r="C35" s="64">
-        <f>SUM(C9:C13)</f>
-        <v>97050.562896637624</v>
-      </c>
+      <c r="B35" s="60" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" s="63">
+        <f>SUM(C25:C28)</f>
+        <v>1580000</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F35" s="25"/>
+      <c r="H35" s="3"/>
       <c r="I35"/>
       <c r="K35"/>
       <c r="L35"/>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B36" s="53" t="s">
-        <v>106</v>
-      </c>
-      <c r="C36" s="65">
-        <f>SUM(C16:C19,C6)</f>
-        <v>243744</v>
+      <c r="B36" s="49" t="s">
+        <v>107</v>
+      </c>
+      <c r="C36" s="64">
+        <f>SUM(C9:C13)</f>
+        <v>97050.562896637624</v>
       </c>
       <c r="I36"/>
       <c r="K36"/>
       <c r="L36"/>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B37" s="66" t="s">
-        <v>10</v>
-      </c>
-      <c r="C37" s="67">
-        <f>SUM(L31)</f>
-        <v>156573.33086193868</v>
+      <c r="B37" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="C37" s="65">
+        <f>SUM(C16:C19,C6)</f>
+        <v>257469.9</v>
       </c>
       <c r="I37"/>
       <c r="K37"/>
       <c r="L37"/>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B38" s="55" t="s">
-        <v>109</v>
-      </c>
-      <c r="C38" s="56">
-        <f>SUM(I31)</f>
-        <v>71762.640724159399</v>
+      <c r="B38" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="67">
+        <f>SUM(L32)</f>
+        <v>156573.33086193868</v>
       </c>
       <c r="I38"/>
       <c r="K38"/>
       <c r="L38"/>
     </row>
-    <row r="39" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C39" s="9" t="s">
-        <v>33</v>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B39" s="55" t="s">
+        <v>109</v>
+      </c>
+      <c r="C39" s="56">
+        <f>SUM(I32)</f>
+        <v>71762.640724159399</v>
       </c>
       <c r="I39"/>
       <c r="K39"/>
       <c r="L39"/>
     </row>
     <row r="40" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B40" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="C40" s="68">
-        <f>SUM(C34:C38)</f>
-        <v>2149130.5344827357</v>
+      <c r="C40" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="I40"/>
       <c r="K40"/>
       <c r="L40"/>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B41" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="C41" s="68">
+        <f>SUM(C35:C39)</f>
+        <v>2162856.4344827356</v>
+      </c>
       <c r="I41"/>
       <c r="K41"/>
       <c r="L41"/>
@@ -9425,6 +9449,11 @@
       <c r="I42"/>
       <c r="K42"/>
       <c r="L42"/>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="I43"/>
+      <c r="K43"/>
+      <c r="L43"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -9952,7 +9981,7 @@
       <c r="I30"/>
       <c r="K30"/>
       <c r="L30" s="42">
-        <f>'kalte NW'!L31</f>
+        <f>'kalte NW'!L32</f>
         <v>156573.33086193868</v>
       </c>
       <c r="M30" s="80" t="s">

</xml_diff>